<commit_message>
Bondora: switch to English website
</commit_message>
<xml_diff>
--- a/tests/input/input_test_bondora_parser_missing_month.xlsx
+++ b/tests/input/input_test_bondora_parser_missing_month.xlsx
@@ -22,37 +22,37 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
-    <t xml:space="preserve">Zeitraum</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Startguthaben</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Eingesetztes Kapital (netto)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Investitionen (netto)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Erhaltener Kapitalbetrag - gesamt</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Erhaltene Zinsen - gesamt</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Darlehensbetrag und erhaltene Zinsen - insgesamt</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Endsaldo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Geplanter Kapitalbetrag - gesamt</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Geplante Zinsen - gesamt</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Kapitalbetrag und geplante Zinsen - gesamt</t>
+    <t xml:space="preserve">Period</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Opening balance</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Net capital deployed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Net loan investments</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Principal received - total</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Interest received - total</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Principal and interest received - total</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Closing balance</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Principal planned - total</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Interest planned - total</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Principal and interest planned - total</t>
   </si>
 </sst>
 </file>
@@ -103,19 +103,12 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thin"/>
       <diagonal/>
     </border>
   </borders>
@@ -153,8 +146,8 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
@@ -181,7 +174,7 @@
   <dimension ref="A1:K1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B10" activeCellId="0" sqref="B10"/>
+      <selection pane="topLeft" activeCell="D6" activeCellId="2" sqref="E1:G1 I1:K1 D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -200,7 +193,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="12" style="0" width="8.67"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>

</xml_diff>